<commit_message>
Añadir funciones de comparación de palabras y frases exactas
</commit_message>
<xml_diff>
--- a/docs/example 2.xlsx
+++ b/docs/example 2.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Mi unidad\1. IRM Analytics\2. MERCURIO\6. FREELANCERS\20240430 ENTIDADES DUPLICADAS\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97F50838-B53B-4A67-BB2E-21330150C36C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="108">
   <si>
     <t>Pedro Sanchez</t>
   </si>
@@ -160,12 +154,201 @@
   </si>
   <si>
     <t>F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pedro Sánchez </t>
+  </si>
+  <si>
+    <t>0 0 0</t>
+  </si>
+  <si>
+    <t>14 13 14</t>
+  </si>
+  <si>
+    <t>12 11 12</t>
+  </si>
+  <si>
+    <t>29 29 31</t>
+  </si>
+  <si>
+    <t>13 12 13</t>
+  </si>
+  <si>
+    <t>23 23 23</t>
+  </si>
+  <si>
+    <t>16 16 16</t>
+  </si>
+  <si>
+    <t>19 16 17</t>
+  </si>
+  <si>
+    <t>43 42 43</t>
+  </si>
+  <si>
+    <t>16 15 16</t>
+  </si>
+  <si>
+    <t>31 31 33</t>
+  </si>
+  <si>
+    <t>13 11 12</t>
+  </si>
+  <si>
+    <t>69 45 45</t>
+  </si>
+  <si>
+    <t>14 7 8</t>
+  </si>
+  <si>
+    <t>8 8 8</t>
+  </si>
+  <si>
+    <t>19 18 20</t>
+  </si>
+  <si>
+    <t>28 16 17</t>
+  </si>
+  <si>
+    <t>23 21 22</t>
+  </si>
+  <si>
+    <t>21 21 21</t>
+  </si>
+  <si>
+    <t>14 14 14</t>
+  </si>
+  <si>
+    <t>13 13 13</t>
+  </si>
+  <si>
+    <t>38 15 15</t>
+  </si>
+  <si>
+    <t>18 8 8</t>
+  </si>
+  <si>
+    <t>11 10 11</t>
+  </si>
+  <si>
+    <t>15 15 15</t>
+  </si>
+  <si>
+    <t>7 7 7</t>
+  </si>
+  <si>
+    <t>39 37 37</t>
+  </si>
+  <si>
+    <t>9 9 9</t>
+  </si>
+  <si>
+    <t>15 13 14</t>
+  </si>
+  <si>
+    <t>29 28 29</t>
+  </si>
+  <si>
+    <t>25 23 23</t>
+  </si>
+  <si>
+    <t>37 37 37</t>
+  </si>
+  <si>
+    <t>56 54 55</t>
+  </si>
+  <si>
+    <t>11 11 11</t>
+  </si>
+  <si>
+    <t>2 1 2</t>
+  </si>
+  <si>
+    <t>12 12 12</t>
+  </si>
+  <si>
+    <t>10 10 10</t>
+  </si>
+  <si>
+    <t>31 30 33</t>
+  </si>
+  <si>
+    <t>25 24 25</t>
+  </si>
+  <si>
+    <t>18 17 18</t>
+  </si>
+  <si>
+    <t>17 15 15</t>
+  </si>
+  <si>
+    <t>41 41 41</t>
+  </si>
+  <si>
+    <t>33 32 35</t>
+  </si>
+  <si>
+    <t>11 10 10</t>
+  </si>
+  <si>
+    <t>71 46 47</t>
+  </si>
+  <si>
+    <t>12 6 6</t>
+  </si>
+  <si>
+    <t>10 9 10</t>
+  </si>
+  <si>
+    <t>21 19 22</t>
+  </si>
+  <si>
+    <t>26 15 15</t>
+  </si>
+  <si>
+    <t>21 20 20</t>
+  </si>
+  <si>
+    <t>23 22 23</t>
+  </si>
+  <si>
+    <t>15 14 15</t>
+  </si>
+  <si>
+    <t>40 16 17</t>
+  </si>
+  <si>
+    <t>20 9 10</t>
+  </si>
+  <si>
+    <t>17 16 17</t>
+  </si>
+  <si>
+    <t>9 8 9</t>
+  </si>
+  <si>
+    <t>41 38 39</t>
+  </si>
+  <si>
+    <t>13 12 12</t>
+  </si>
+  <si>
+    <t>27 27 27</t>
+  </si>
+  <si>
+    <t>27 24 25</t>
+  </si>
+  <si>
+    <t>39 38 39</t>
+  </si>
+  <si>
+    <t>54 53 53</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -472,23 +655,28 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C41"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="70.5703125" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>40</v>
       </c>
@@ -499,7 +687,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>11742</v>
       </c>
@@ -509,8 +697,21 @@
       <c r="C2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J2" t="str">
+        <f>""""&amp;B2&amp;""""&amp;","</f>
+        <v>"Pedro Sanchez",</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>79085</v>
       </c>
@@ -520,8 +721,18 @@
       <c r="C3" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E3" t="s">
+        <v>81</v>
+      </c>
+      <c r="J3" t="str">
+        <f t="shared" ref="J3:J41" si="0">""""&amp;B3&amp;""""&amp;","</f>
+        <v>"Gobierno de Pedro Sánchez",</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>79271</v>
       </c>
@@ -531,8 +742,18 @@
       <c r="C4" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="D4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" t="s">
+        <v>82</v>
+      </c>
+      <c r="J4" t="str">
+        <f t="shared" si="0"/>
+        <v>"Esposa de Pedro Sánchez",</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>86683</v>
       </c>
@@ -542,8 +763,18 @@
       <c r="C5" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" t="s">
+        <v>83</v>
+      </c>
+      <c r="J5" t="str">
+        <f t="shared" si="0"/>
+        <v>"pantuflas para los pies de pedro sanchez",</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>92046</v>
       </c>
@@ -553,8 +784,18 @@
       <c r="C6" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="D6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E6" t="s">
+        <v>79</v>
+      </c>
+      <c r="J6" t="str">
+        <f t="shared" si="0"/>
+        <v>"Presidente Pedro Sánchez",</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>99394</v>
       </c>
@@ -564,8 +805,18 @@
       <c r="C7" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="D7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E7" t="s">
+        <v>84</v>
+      </c>
+      <c r="J7" t="str">
+        <f t="shared" si="0"/>
+        <v>"Spanish Prime Minister Pedro Sanchez",</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>123046</v>
       </c>
@@ -575,8 +826,18 @@
       <c r="C8" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="D8" t="s">
+        <v>52</v>
+      </c>
+      <c r="E8" t="s">
+        <v>85</v>
+      </c>
+      <c r="J8" t="str">
+        <f t="shared" si="0"/>
+        <v>"Criticas contra Pedro Sanchez",</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>124400</v>
       </c>
@@ -586,8 +847,18 @@
       <c r="C9" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="D9" t="s">
+        <v>53</v>
+      </c>
+      <c r="E9" t="s">
+        <v>86</v>
+      </c>
+      <c r="J9" t="str">
+        <f t="shared" si="0"/>
+        <v>"Pedro Sánchez Pérez-Castejón",</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>128389</v>
       </c>
@@ -597,8 +868,18 @@
       <c r="C10" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D10" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" t="s">
+        <v>87</v>
+      </c>
+      <c r="J10" t="str">
+        <f t="shared" si="0"/>
+        <v>"Pedro Sánchez, Kajsa Ollongren y mandatarios de Europa",</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>129867</v>
       </c>
@@ -608,8 +889,18 @@
       <c r="C11" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="D11" t="s">
+        <v>50</v>
+      </c>
+      <c r="E11" t="s">
+        <v>79</v>
+      </c>
+      <c r="J11" t="str">
+        <f t="shared" si="0"/>
+        <v>"Partido de Pedro Sánchez",</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>133048</v>
       </c>
@@ -619,8 +910,18 @@
       <c r="C12" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="D12" t="s">
+        <v>55</v>
+      </c>
+      <c r="E12" t="s">
+        <v>65</v>
+      </c>
+      <c r="J12" t="str">
+        <f t="shared" si="0"/>
+        <v>"estrategia de Pedro Sánchez",</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>145035</v>
       </c>
@@ -630,8 +931,18 @@
       <c r="C13" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="D13" t="s">
+        <v>56</v>
+      </c>
+      <c r="E13" t="s">
+        <v>88</v>
+      </c>
+      <c r="J13" t="str">
+        <f t="shared" si="0"/>
+        <v>"allies of bruised spanish pm pedro sanchez",</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>153161</v>
       </c>
@@ -641,8 +952,18 @@
       <c r="C14" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="D14" t="s">
+        <v>57</v>
+      </c>
+      <c r="E14" t="s">
+        <v>89</v>
+      </c>
+      <c r="J14" t="str">
+        <f t="shared" si="0"/>
+        <v>"Pedro Sánchez Fernández",</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>153602</v>
       </c>
@@ -652,8 +973,18 @@
       <c r="C15" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D15" t="s">
+        <v>58</v>
+      </c>
+      <c r="E15" t="s">
+        <v>90</v>
+      </c>
+      <c r="J15" t="str">
+        <f t="shared" si="0"/>
+        <v>"Педро Санчес Перес-Кастехон (Pedro Sanchez Perez-Castejon)",</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>153610</v>
       </c>
@@ -663,8 +994,18 @@
       <c r="C16" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D16" t="s">
+        <v>59</v>
+      </c>
+      <c r="E16" t="s">
+        <v>91</v>
+      </c>
+      <c r="J16" t="str">
+        <f t="shared" si="0"/>
+        <v>"桑切斯 (Pedro Sánchez)",</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>154118</v>
       </c>
@@ -674,8 +1015,18 @@
       <c r="C17" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="D17" t="s">
+        <v>60</v>
+      </c>
+      <c r="E17" t="s">
+        <v>92</v>
+      </c>
+      <c r="J17" t="str">
+        <f t="shared" si="0"/>
+        <v>"Wife of Pedro Sanchez",</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>154380</v>
       </c>
@@ -685,8 +1036,18 @@
       <c r="C18" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="D18" t="s">
+        <v>51</v>
+      </c>
+      <c r="E18" t="s">
+        <v>84</v>
+      </c>
+      <c r="J18" t="str">
+        <f t="shared" si="0"/>
+        <v>"Spain's Prime Minister Pedro Sanchez",</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>155512</v>
       </c>
@@ -696,8 +1057,18 @@
       <c r="C19" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="D19" t="s">
+        <v>61</v>
+      </c>
+      <c r="E19" t="s">
+        <v>93</v>
+      </c>
+      <c r="J19" t="str">
+        <f t="shared" si="0"/>
+        <v>"otros pedro sanchez en España",</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>156220</v>
       </c>
@@ -707,8 +1078,18 @@
       <c r="C20" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="D20" t="s">
+        <v>62</v>
+      </c>
+      <c r="E20" t="s">
+        <v>94</v>
+      </c>
+      <c r="J20" t="str">
+        <f t="shared" si="0"/>
+        <v>"Педро Санчес (Pedro Sánchez)",</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>156968</v>
       </c>
@@ -718,8 +1099,18 @@
       <c r="C21" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="D21" t="s">
+        <v>63</v>
+      </c>
+      <c r="E21" t="s">
+        <v>95</v>
+      </c>
+      <c r="J21" t="str">
+        <f t="shared" si="0"/>
+        <v>"Partido Político de Pedro Sánchez",</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>157126</v>
       </c>
@@ -729,8 +1120,18 @@
       <c r="C22" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="D22" t="s">
+        <v>64</v>
+      </c>
+      <c r="E22" t="s">
+        <v>96</v>
+      </c>
+      <c r="J22" t="str">
+        <f t="shared" si="0"/>
+        <v>"Pedro Sanchez's wife, Begona Gomez",</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>157636</v>
       </c>
@@ -740,8 +1141,18 @@
       <c r="C23" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="D23" t="s">
+        <v>65</v>
+      </c>
+      <c r="E23" t="s">
+        <v>55</v>
+      </c>
+      <c r="J23" t="str">
+        <f t="shared" si="0"/>
+        <v>"Pedro Sanchez, Begona Gomez",</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>157768</v>
       </c>
@@ -751,8 +1162,18 @@
       <c r="C24" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="D24" t="s">
+        <v>66</v>
+      </c>
+      <c r="E24" t="s">
+        <v>97</v>
+      </c>
+      <c r="J24" t="str">
+        <f t="shared" si="0"/>
+        <v>"Pedro Sanchez and his wife",</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>158191</v>
       </c>
@@ -762,8 +1183,18 @@
       <c r="C25" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D25" t="s">
+        <v>67</v>
+      </c>
+      <c r="E25" t="s">
+        <v>98</v>
+      </c>
+      <c r="J25" t="str">
+        <f t="shared" si="0"/>
+        <v>"西班牙首相佩德罗·桑切斯 (Pedro Sanchez)",</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>158209</v>
       </c>
@@ -773,8 +1204,18 @@
       <c r="C26" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="D26" t="s">
+        <v>59</v>
+      </c>
+      <c r="E26" t="s">
+        <v>91</v>
+      </c>
+      <c r="J26" t="str">
+        <f t="shared" si="0"/>
+        <v>"桑杰士 (Pedro Sánchez)",</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>158819</v>
       </c>
@@ -784,8 +1225,18 @@
       <c r="C27" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D27" t="s">
+        <v>68</v>
+      </c>
+      <c r="E27" t="s">
+        <v>99</v>
+      </c>
+      <c r="J27" t="str">
+        <f t="shared" si="0"/>
+        <v>"总理桑杰士 (Pedro Sanchez)",</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>165263</v>
       </c>
@@ -795,8 +1246,18 @@
       <c r="C28" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="D28" t="s">
+        <v>69</v>
+      </c>
+      <c r="E28" t="s">
+        <v>73</v>
+      </c>
+      <c r="J28" t="str">
+        <f t="shared" si="0"/>
+        <v>"Mujer de Pedro Sánchez",</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>165469</v>
       </c>
@@ -806,8 +1267,18 @@
       <c r="C29" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D29" t="s">
+        <v>70</v>
+      </c>
+      <c r="E29" t="s">
+        <v>100</v>
+      </c>
+      <c r="J29" t="str">
+        <f t="shared" si="0"/>
+        <v>"Spanish Leader Pedro Sanchez",</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>165553</v>
       </c>
@@ -817,8 +1288,18 @@
       <c r="C30" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="D30" t="s">
+        <v>71</v>
+      </c>
+      <c r="E30" t="s">
+        <v>101</v>
+      </c>
+      <c r="J30" t="str">
+        <f t="shared" si="0"/>
+        <v>"Pedro Sanchez's wife",</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>165576</v>
       </c>
@@ -828,8 +1309,18 @@
       <c r="C31" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D31" t="s">
+        <v>72</v>
+      </c>
+      <c r="E31" t="s">
+        <v>102</v>
+      </c>
+      <c r="J31" t="str">
+        <f t="shared" si="0"/>
+        <v>"Supporters of Spain’s Prime Minister Pedro Sanchez",</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>165684</v>
       </c>
@@ -839,8 +1330,18 @@
       <c r="C32" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D32" t="s">
+        <v>73</v>
+      </c>
+      <c r="E32" t="s">
+        <v>69</v>
+      </c>
+      <c r="J32" t="str">
+        <f t="shared" si="0"/>
+        <v>"Spain PM Pedro Sanchez",</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>165810</v>
       </c>
@@ -850,8 +1351,18 @@
       <c r="C33" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="D33" t="s">
+        <v>74</v>
+      </c>
+      <c r="E33" t="s">
+        <v>103</v>
+      </c>
+      <c r="J33" t="str">
+        <f t="shared" si="0"/>
+        <v>"Dimisión de Pedro Sánchez",</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>166350</v>
       </c>
@@ -861,8 +1372,18 @@
       <c r="C34" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="D34" t="s">
+        <v>75</v>
+      </c>
+      <c r="E34" t="s">
+        <v>104</v>
+      </c>
+      <c r="J34" t="str">
+        <f t="shared" si="0"/>
+        <v>"Longevidad del gobierno de Pedro Sánchez",</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>166532</v>
       </c>
@@ -872,8 +1393,18 @@
       <c r="C35" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="D35" t="s">
+        <v>70</v>
+      </c>
+      <c r="E35" t="s">
+        <v>100</v>
+      </c>
+      <c r="J35" t="str">
+        <f t="shared" si="0"/>
+        <v>"Prime Minister Pedro Sanchez",</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>167298</v>
       </c>
@@ -883,8 +1414,18 @@
       <c r="C36" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="D36" t="s">
+        <v>76</v>
+      </c>
+      <c r="E36" t="s">
+        <v>105</v>
+      </c>
+      <c r="J36" t="str">
+        <f t="shared" si="0"/>
+        <v>"Spain’s Prime Minister Pedro Sanchez",</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>168061</v>
       </c>
@@ -894,8 +1435,18 @@
       <c r="C37" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="D37" t="s">
+        <v>77</v>
+      </c>
+      <c r="E37" t="s">
+        <v>106</v>
+      </c>
+      <c r="J37" t="str">
+        <f t="shared" si="0"/>
+        <v>"Supporters of Spain's Prime Minister Pedro Sanchez",</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>168345</v>
       </c>
@@ -905,8 +1456,18 @@
       <c r="C38" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="D38" t="s">
+        <v>70</v>
+      </c>
+      <c r="E38" t="s">
+        <v>100</v>
+      </c>
+      <c r="J38" t="str">
+        <f t="shared" si="0"/>
+        <v>"Pedro Sanchez und seine Frau",</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>170963</v>
       </c>
@@ -916,8 +1477,18 @@
       <c r="C39" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="D39" t="s">
+        <v>75</v>
+      </c>
+      <c r="E39" t="s">
+        <v>104</v>
+      </c>
+      <c r="J39" t="str">
+        <f t="shared" si="0"/>
+        <v>"allegations against Pedro Sánchez's wife",</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>171233</v>
       </c>
@@ -927,8 +1498,18 @@
       <c r="C40" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D40" t="s">
+        <v>78</v>
+      </c>
+      <c r="E40" t="s">
+        <v>107</v>
+      </c>
+      <c r="J40" t="str">
+        <f t="shared" si="0"/>
+        <v>"Hija del juez que aceptó querella contra la mujer de Pedro Sánchez",</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>174730</v>
       </c>
@@ -938,8 +1519,21 @@
       <c r="C41" t="s">
         <v>43</v>
       </c>
-    </row>
+      <c r="D41" t="s">
+        <v>79</v>
+      </c>
+      <c r="E41" t="s">
+        <v>50</v>
+      </c>
+      <c r="J41" t="str">
+        <f t="shared" si="0"/>
+        <v>"Spanish PM Pedro Sanchez",</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>